<commit_message>
v1.1 Review the system constraints and closed the reviewed notifications CRS
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D704A52-A00A-40DE-8A76-8FCF3BB7930F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -74,9 +75,6 @@
   </si>
   <si>
     <t>V1.1</t>
-  </si>
-  <si>
-    <t>open</t>
   </si>
   <si>
     <t>LH_CRS_NOTIFICATION_Review_001</t>
@@ -110,13 +108,47 @@
   </si>
   <si>
     <t>review the notification feature and ask for some updates on it</t>
+  </si>
+  <si>
+    <t>not applicable</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>21/4/2025</t>
+  </si>
+  <si>
+    <t>LH_CRS_SYSTEM_Review_003</t>
+  </si>
+  <si>
+    <t>Omar Sherif</t>
+  </si>
+  <si>
+    <t>V1.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO comments  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A
+</t>
+  </si>
+  <si>
+    <t>Ahmed Abouzied</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>review the system constraints and closed the reviewd notifications CRS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,8 +191,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,6 +229,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -273,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -281,7 +325,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -299,34 +343,28 @@
     <xf numFmtId="15" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -601,128 +639,158 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="15" customWidth="1"/>
-    <col min="5" max="5" width="77.5703125" style="15" customWidth="1"/>
-    <col min="6" max="6" width="38.5703125" style="15" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="77.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="38.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="11" customFormat="1" ht="18.75">
+    <row r="1" spans="1:9" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="84.75" customHeight="1">
+    <row r="2" spans="1:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>21</v>
+      <c r="G2" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" ht="120">
+    <row r="3" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>21</v>
-      </c>
       <c r="H3" s="13" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="I3" s="16"/>
     </row>
-    <row r="10" spans="1:9">
-      <c r="G10" s="15" t="s">
-        <v>24</v>
+    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G10" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I2:I3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I2:I4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -731,22 +799,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="48.6640625" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25">
+    <row r="1" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -760,27 +828,36 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="37.5">
+    <row r="2" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="D2" s="8">
         <v>45764</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
+    <row r="3" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="8">
+        <v>45768</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
review the login and No Comments
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D704A52-A00A-40DE-8A76-8FCF3BB7930F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -142,13 +141,34 @@
   </si>
   <si>
     <t>review the system constraints and closed the reviewd notifications CRS</t>
+  </si>
+  <si>
+    <t>v1.2</t>
+  </si>
+  <si>
+    <t>Hala Eldaly</t>
+  </si>
+  <si>
+    <t>29/4/2025</t>
+  </si>
+  <si>
+    <t>LH_CRS_LOGIN_Review_004</t>
+  </si>
+  <si>
+    <t>V1.9</t>
+  </si>
+  <si>
+    <t>Gehad Ashry</t>
+  </si>
+  <si>
+    <t>review the login and No Comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -646,28 +666,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="77.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="38.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="77.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="38.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="12" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="12" customFormat="1" ht="18.75">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -696,7 +716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="84.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -723,7 +743,7 @@
       </c>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="90">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -750,7 +770,7 @@
       </c>
       <c r="I3" s="16"/>
     </row>
-    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="45">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
@@ -779,7 +799,36 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="45">
+      <c r="A5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="G10" s="1" t="s">
         <v>23</v>
       </c>
@@ -787,10 +836,10 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I2:I4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I2:I5">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H4" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H5">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -799,22 +848,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="48.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="20.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -828,7 +877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="37.5">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -842,7 +891,7 @@
         <v>45764</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="37.5">
       <c r="A3" s="6" t="s">
         <v>37</v>
       </c>
@@ -854,6 +903,20 @@
       </c>
       <c r="D3" s="8">
         <v>45768</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75">
+      <c r="A4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="8">
+        <v>45776</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.3 review the user home page
review the user home page and ask to modify some of them
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -76,99 +76,117 @@
     <t>V1.1</t>
   </si>
   <si>
-    <t>LH_CRS_NOTIFICATION_Review_001</t>
-  </si>
-  <si>
-    <t>LH_CRS_NOTIFICATION_Review_002</t>
+    <t>open</t>
   </si>
   <si>
     <t>Omar</t>
   </si>
   <si>
-    <t>At the notification feature the first crs need to be more atomic to contain only one 
-action the user could do</t>
-  </si>
-  <si>
-    <t xml:space="preserve">make the CRS is as follow""Users can follow and unfollow specific categories."
-</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">At notification feature the CRS is too vauge and does not explain what the customer want the system do </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eman </t>
+  </si>
+  <si>
+    <t>review the notification feature and ask for some updates on it</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>30/4/2025</t>
+  </si>
+  <si>
+    <t>Reviewed Entity</t>
+  </si>
+  <si>
+    <t>LH-CRS-NOTIFICATION-001</t>
+  </si>
+  <si>
+    <t>LH-CRS-NOTIFICATION-002</t>
+  </si>
+  <si>
+    <t>LH-CRS-USERHOME-002</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-001</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-002</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-003</t>
+  </si>
+  <si>
+    <t>Ahmed Abuzaid</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>v1.2</t>
+  </si>
+  <si>
+    <t>v1.3</t>
+  </si>
+  <si>
+    <t>v1.11</t>
+  </si>
+  <si>
+    <t>in this CRS you mention a lot of detalies that will not inmportant for the customer and it can be a SRS</t>
+  </si>
+  <si>
+    <t>At the notification feature the first crs need to be more atomic to contain only one action the user could do</t>
+  </si>
+  <si>
+    <t>make the CRS is as follow""Users can follow and unfollow specific categories."</t>
   </si>
   <si>
     <t xml:space="preserve">write the CRS as this"The system must notify users within the website interface when new content is added to a followed category."
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Eman </t>
-  </si>
-  <si>
-    <t>review the notification feature and ask for some updates on it</t>
-  </si>
-  <si>
-    <t>not applicable</t>
-  </si>
-  <si>
-    <t>closed</t>
-  </si>
-  <si>
-    <t>21/4/2025</t>
-  </si>
-  <si>
-    <t>LH_CRS_SYSTEM_Review_003</t>
-  </si>
-  <si>
-    <t>Omar Sherif</t>
-  </si>
-  <si>
-    <t>V1.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO comments  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">N/A
-</t>
-  </si>
-  <si>
-    <t>Ahmed Abouzied</t>
-  </si>
-  <si>
-    <t>v1.1</t>
-  </si>
-  <si>
-    <t>review the system constraints and closed the reviewd notifications CRS</t>
-  </si>
-  <si>
-    <t>v1.2</t>
+    <t>it can only be "The home page must dynamically fetch and display notifications for new articles in categories the user follows"</t>
+  </si>
+  <si>
+    <t>hala</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-004</t>
+  </si>
+  <si>
+    <t>LH-CRS-USERHOME-003</t>
+  </si>
+  <si>
+    <t>it can only be "Posts from followed categories must be listed on the user home page"</t>
+  </si>
+  <si>
+    <t>in this CRS you mention a lot of detalies that will not important for the customer and it can be a SRS</t>
+  </si>
+  <si>
+    <t>omar sherif</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Review the system constraints and closed the reviewed notifications CRS</t>
+  </si>
+  <si>
+    <t>review the login and No Comments</t>
   </si>
   <si>
     <t>Hala Eldaly</t>
   </si>
   <si>
-    <t>29/4/2025</t>
-  </si>
-  <si>
-    <t>LH_CRS_LOGIN_Review_004</t>
-  </si>
-  <si>
-    <t>V1.9</t>
-  </si>
-  <si>
-    <t>Gehad Ashry</t>
-  </si>
-  <si>
-    <t>review the login and No Comments</t>
+    <t>review the user home page and ask to modify some of them</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,14 +229,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,14 +261,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -318,26 +324,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -345,9 +336,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -363,29 +351,41 @@
     <xf numFmtId="15" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -447,7 +447,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -482,7 +482,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -667,179 +667,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="77.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="38.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="18.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="66.140625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="45.5703125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="12" customFormat="1" ht="18.75">
+    <row r="1" spans="1:10" s="10" customFormat="1" ht="18.75">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="84.75" customHeight="1">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:10" ht="30">
+      <c r="A2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="60">
+      <c r="A3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="45">
+      <c r="A4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="9" t="s">
+      <c r="J4" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30">
+      <c r="A5" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="H9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="14"/>
-    </row>
-    <row r="3" spans="1:9" ht="90">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="16"/>
-    </row>
-    <row r="4" spans="1:9" ht="45">
-      <c r="A4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="45">
-      <c r="A5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="G10" s="1" t="s">
-        <v>23</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="I2:I5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J3">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="H2:H5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I3">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -849,10 +868,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -864,63 +883,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="37.5">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="8">
+      <c r="B2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="7">
         <v>45764</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="37.5">
-      <c r="A3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="8">
+    <row r="3" spans="1:4" ht="56.25">
+      <c r="A3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="7">
         <v>45768</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75">
-      <c r="A4" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="8">
+      <c r="A4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="7">
         <v>45776</v>
       </c>
     </row>
+    <row r="5" spans="1:4" ht="37.5">
+      <c r="A5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="7">
+        <v>45777</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v1.4 Reviewed Admin Constraints (Deleting Post) feature
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AFB50E-61E8-4787-86B0-C513695E9766}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
   <si>
     <t>ID</t>
   </si>
@@ -82,9 +83,6 @@
     <t>Omar</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t xml:space="preserve">At notification feature the CRS is too vauge and does not explain what the customer want the system do </t>
   </si>
   <si>
@@ -131,9 +129,6 @@
   </si>
   <si>
     <t>v1.3</t>
-  </si>
-  <si>
-    <t>v1.11</t>
   </si>
   <si>
     <t>in this CRS you mention a lot of detalies that will not inmportant for the customer and it can be a SRS</t>
@@ -180,13 +175,219 @@
   </si>
   <si>
     <t>review the user home page and ask to modify some of them</t>
+  </si>
+  <si>
+    <t>v1.4</t>
+  </si>
+  <si>
+    <t>Gehad Ashry</t>
+  </si>
+  <si>
+    <t>v2.0</t>
+  </si>
+  <si>
+    <t>v2.1</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-005</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-006</t>
+  </si>
+  <si>
+    <t>LH-CRS-DELETEPOST-001</t>
+  </si>
+  <si>
+    <t>LH-CRS-DELETEPOST-002</t>
+  </si>
+  <si>
+    <t>Watch out for grammatical errors and typos that may reduce clarity.</t>
+  </si>
+  <si>
+    <t>This sentence is grammatically incorrect and slightly confusing in its current form. The phrase "searching about posts" should be revised for clarity, and "its username" should be "their username" since it refers to a user.</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-007</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-008</t>
+  </si>
+  <si>
+    <t>LH-CRS-DELETEPOST-003</t>
+  </si>
+  <si>
+    <t>Try rewording it to better reflect the case where a user exists but has no posts.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Replace with</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: "The admin has the ability to delete any post (articles, videos, or audio recordings) through the 'Delete Post' page."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Replace with</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: "The admin can delete a post by searching for a user's posts using their username."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Replace with</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: "If no posts are found for the entered username, an informative message must be displayed."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This sentence is also unclear and repeats part of the previous requirement. If the system handles both "no posts" and "user not found" cases differently, clarify each. Otherwise, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>you might consider combining them.</t>
+    </r>
+  </si>
+  <si>
+    <t>LH-CRS-DELETEPOST-004</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Combine</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> both of (003 &amp; 004) but if the system handles them differently </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Replace with: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"If the entered username does not exist in the system, an informative message must be displayed."</t>
+    </r>
+  </si>
+  <si>
+    <t>LH-CRS-DELETEPOST-005</t>
+  </si>
+  <si>
+    <t>This sentence is mostly clear, but there's a typo in "pf" (should be "of"). Also, consider rewording slightly to improve tone and flow.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Replace with: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"The admin can return to the admin home page by clicking the website logo."</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">review Admin Constraints for Deleting Post feature </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +429,22 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -328,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -366,9 +583,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -377,9 +591,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -666,11 +877,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -681,8 +892,8 @@
     <col min="4" max="4" width="22.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" style="12" customWidth="1"/>
     <col min="6" max="6" width="66.140625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="45.5703125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.85546875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" style="12" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="12"/>
@@ -696,7 +907,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>1</v>
@@ -721,14 +932,14 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="30">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>15</v>
@@ -736,78 +947,78 @@
       <c r="E2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>40</v>
+      <c r="F2" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>38</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="60">
+      <c r="A3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="45">
+      <c r="A4" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="60">
-      <c r="A3" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="16" t="s">
+      <c r="B4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="17" t="s">
+      <c r="D4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="45">
-      <c r="A4" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>18</v>
@@ -817,61 +1028,217 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="30">
-      <c r="A5" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="16" t="s">
+      <c r="A5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="16" t="s">
+      <c r="H5" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="H9" s="12" t="s">
-        <v>20</v>
+    <row r="6" spans="1:10" ht="45">
+      <c r="A6" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="60">
+      <c r="A7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30">
+      <c r="A8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="60">
+      <c r="A9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30">
+      <c r="A10" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I3" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -901,10 +1268,10 @@
         <v>13</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="D2" s="7">
         <v>45764</v>
@@ -912,13 +1279,13 @@
     </row>
     <row r="3" spans="1:4" ht="56.25">
       <c r="A3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" s="7">
         <v>45768</v>
@@ -926,13 +1293,13 @@
     </row>
     <row r="4" spans="1:4" ht="18.75">
       <c r="A4" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D4" s="7">
         <v>45776</v>
@@ -940,15 +1307,29 @@
     </row>
     <row r="5" spans="1:4" ht="37.5">
       <c r="A5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="7">
+        <v>45777</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="37.5">
+      <c r="A6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="7">
+      <c r="C6" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="7">
         <v>45777</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v1.5 modify delete post CRS& review publish audio
1/modify delete post CRSs according to reviewer cooments
2/review publish audio CRSs, add my comments , ask for some modifications
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AFB50E-61E8-4787-86B0-C513695E9766}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="88">
   <si>
     <t>ID</t>
   </si>
@@ -382,11 +381,52 @@
   <si>
     <t xml:space="preserve">review Admin Constraints for Deleting Post feature </t>
   </si>
+  <si>
+    <t>v1.5</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISHAUDIO-001</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISHAUDIO-002</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISHAUDIO-003</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-009</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-010</t>
+  </si>
+  <si>
+    <t>v2.2</t>
+  </si>
+  <si>
+    <t>it can be: "Only registered and logged-in users can access the audio publishing interface that found in a publish drop down in categories page"</t>
+  </si>
+  <si>
+    <t>this CRS contain a lot of details that might be important in SRS not here
+and it can more simple and to the point</t>
+  </si>
+  <si>
+    <t>it can be: "Only registered and logged-in users can recored a voice note and set a title for it then publish it "</t>
+  </si>
+  <si>
+    <t>you mentioned that the audio recorde will have two limits "one for duration of record and another for its size" ,but I think we can only suffice with only duration as the 5 minutes audio recorde ussaully doesn't exceeds 20 MB</t>
+  </si>
+  <si>
+    <t>it can be: "The user can record a voice message for up to 5 minutes. If the time limit is exceeded,a message will appear explaining this."</t>
+  </si>
+  <si>
+    <t>1/modify delete post CRSs according to reviewer cooments
+2/review publish audio CRSs, add my comments , ask for some modifications</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -877,11 +917,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1085,7 +1125,7 @@
         <v>32</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="J6" s="11" t="s">
         <v>18</v>
@@ -1117,7 +1157,7 @@
         <v>32</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="J7" s="15" t="s">
         <v>18</v>
@@ -1149,7 +1189,7 @@
         <v>32</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>18</v>
@@ -1181,7 +1221,7 @@
         <v>32</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="J9" s="15" t="s">
         <v>18</v>
@@ -1213,18 +1253,114 @@
         <v>32</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>18</v>
       </c>
     </row>
+    <row r="11" spans="1:10" ht="45">
+      <c r="A11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30">
+      <c r="A12" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="60">
+      <c r="A13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J3" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J3">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I3" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I3">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1234,18 +1370,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.85546875" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+    <col min="3" max="3" width="68.42578125" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1333,6 +1469,20 @@
         <v>45777</v>
       </c>
     </row>
+    <row r="7" spans="1:4" ht="93.75">
+      <c r="A7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="7">
+        <v>45777</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
v1.6 Reviewed Publish article CRS
LH_CRS_PUBLISHARTICLE_Review_043
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EABDCD2-69D1-45B9-8112-C6E9FAE75D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7650"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="96">
   <si>
     <t>ID</t>
   </si>
@@ -422,12 +423,36 @@
     <t>1/modify delete post CRSs according to reviewer cooments
 2/review publish audio CRSs, add my comments , ask for some modifications</t>
   </si>
+  <si>
+    <t>30/4/2026</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-011</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISHARTICLE-003</t>
+  </si>
+  <si>
+    <t>Mahmoud Abdelmageed</t>
+  </si>
+  <si>
+    <t>The maximum words limit is not shown to the user</t>
+  </si>
+  <si>
+    <t>clarify that the maximum words should be visible to the user in the counter as shown in the wireframe</t>
+  </si>
+  <si>
+    <t>v1.6</t>
+  </si>
+  <si>
+    <t>Reviewed Publish article CRS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -482,6 +507,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -585,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -617,26 +648,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -917,29 +957,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="12" customWidth="1"/>
-    <col min="6" max="6" width="66.140625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="55.85546875" style="12" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="66.109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="55.88671875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" style="12" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="10" customFormat="1" ht="18.75">
+    <row r="1" spans="1:10" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -971,7 +1011,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30">
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
@@ -1003,7 +1043,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="60">
+    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>14</v>
       </c>
@@ -1035,7 +1075,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="45">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>24</v>
       </c>
@@ -1067,7 +1107,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>24</v>
       </c>
@@ -1099,7 +1139,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="45">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>24</v>
       </c>
@@ -1131,7 +1171,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="60">
+    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>24</v>
       </c>
@@ -1163,7 +1203,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
@@ -1195,7 +1235,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="60">
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>24</v>
       </c>
@@ -1227,7 +1267,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
@@ -1259,7 +1299,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="45">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>24</v>
       </c>
@@ -1291,7 +1331,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="30">
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>24</v>
       </c>
@@ -1323,7 +1363,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="60">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>24</v>
       </c>
@@ -1355,12 +1395,45 @@
         <v>18</v>
       </c>
     </row>
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I3" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1370,22 +1443,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="68.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="68.44140625" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25">
+    <row r="1" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -1399,7 +1472,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="37.5">
+    <row r="2" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
@@ -1413,7 +1486,7 @@
         <v>45764</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="56.25">
+    <row r="3" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>33</v>
       </c>
@@ -1427,7 +1500,7 @@
         <v>45768</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75">
+    <row r="4" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
@@ -1441,7 +1514,7 @@
         <v>45776</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="37.5">
+    <row r="5" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>35</v>
       </c>
@@ -1455,7 +1528,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="37.5">
+    <row r="6" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>51</v>
       </c>
@@ -1469,7 +1542,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="93.75">
+    <row r="7" spans="1:4" ht="74.400000000000006" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>75</v>
       </c>
@@ -1483,7 +1556,22 @@
         <v>45777</v>
       </c>
     </row>
+    <row r="8" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="19">
+        <v>45777</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
v1.7 Reviewed the 'Delete User' feature in the Admin Constraints section
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EABDCD2-69D1-45B9-8112-C6E9FAE75D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="6930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="116">
   <si>
     <t>ID</t>
   </si>
@@ -420,39 +419,103 @@
     <t>it can be: "The user can record a voice message for up to 5 minutes. If the time limit is exceeded,a message will appear explaining this."</t>
   </si>
   <si>
-    <t>1/modify delete post CRSs according to reviewer cooments
+    <t>LH-CRS-Review-011</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISHARTICLE-003</t>
+  </si>
+  <si>
+    <t>Mahmoud Abdelmageed</t>
+  </si>
+  <si>
+    <t>The maximum words limit is not shown to the user</t>
+  </si>
+  <si>
+    <t>clarify that the maximum words should be visible to the user in the counter as shown in the wireframe</t>
+  </si>
+  <si>
+    <t>v1.6</t>
+  </si>
+  <si>
+    <t>Reviewed Publish article CRS</t>
+  </si>
+  <si>
+    <t>v1.7</t>
+  </si>
+  <si>
+    <t>v2.4</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-012</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-013</t>
+  </si>
+  <si>
+    <t>Missed VERSION-HISTORY Modify</t>
+  </si>
+  <si>
+    <t>No name added to owner column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">owner column is empty </t>
+  </si>
+  <si>
+    <t>add your name</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-014</t>
+  </si>
+  <si>
+    <t>LH-CRS-DELETEUSER_001</t>
+  </si>
+  <si>
+    <t>The admin has the ability to delete any user from the delete user page [not delete post page]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spelling mistakes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"ind" → should be "and"  
+"id" → should be "ID"  
+"apear" → should be "appear"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">" delete post" → should be " delete user"  </t>
+  </si>
+  <si>
+    <t>1/modify delete post CRSs according to reviewer comments
 2/review publish audio CRSs, add my comments , ask for some modifications</t>
   </si>
   <si>
-    <t>30/4/2026</t>
-  </si>
-  <si>
-    <t>LH-CRS-Review-011</t>
-  </si>
-  <si>
-    <t>LH-CRS-PUBLISHARTICLE-003</t>
-  </si>
-  <si>
-    <t>Mahmoud Abdelmageed</t>
-  </si>
-  <si>
-    <t>The maximum words limit is not shown to the user</t>
-  </si>
-  <si>
-    <t>clarify that the maximum words should be visible to the user in the counter as shown in the wireframe</t>
-  </si>
-  <si>
-    <t>v1.6</t>
-  </si>
-  <si>
-    <t>Reviewed Publish article CRS</t>
+    <t>LH-CRS-DELETEUSER_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">you don't update version in VERSION-HISTORY </t>
+  </si>
+  <si>
+    <t>You should add [v2.4 update the admin constraints by modifying the delete user constraints]</t>
+  </si>
+  <si>
+    <t>EmanAbusalim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EmanAbusalim
+</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-015</t>
+  </si>
+  <si>
+    <t>Reviewed the 'Delete User' feature in the Admin Constraints section</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -517,8 +580,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -546,6 +616,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -613,10 +695,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -678,8 +761,51 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="9" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -957,29 +1083,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.109375" style="12" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="12" customWidth="1"/>
-    <col min="6" max="6" width="66.109375" style="12" customWidth="1"/>
-    <col min="7" max="7" width="55.88671875" style="12" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" style="12" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="12"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="66.140625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="55.85546875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="10" customFormat="1" ht="18.75">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1011,7 +1137,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="30">
       <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
@@ -1043,7 +1169,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="60">
       <c r="A3" s="14" t="s">
         <v>14</v>
       </c>
@@ -1075,7 +1201,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="45">
       <c r="A4" s="13" t="s">
         <v>24</v>
       </c>
@@ -1107,7 +1233,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="30">
       <c r="A5" s="14" t="s">
         <v>24</v>
       </c>
@@ -1139,7 +1265,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="45">
       <c r="A6" s="13" t="s">
         <v>24</v>
       </c>
@@ -1171,7 +1297,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="60">
       <c r="A7" s="14" t="s">
         <v>24</v>
       </c>
@@ -1203,7 +1329,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="30">
       <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
@@ -1235,7 +1361,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="60">
       <c r="A9" s="14" t="s">
         <v>24</v>
       </c>
@@ -1267,7 +1393,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="30">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
@@ -1299,7 +1425,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="45">
       <c r="A11" s="14" t="s">
         <v>24</v>
       </c>
@@ -1331,7 +1457,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="30">
       <c r="A12" s="13" t="s">
         <v>24</v>
       </c>
@@ -1363,7 +1489,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="60">
       <c r="A13" s="14" t="s">
         <v>24</v>
       </c>
@@ -1395,45 +1521,185 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:10" s="24" customFormat="1" ht="30">
+      <c r="A14" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="D14" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="E14" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="G14" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I14" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="15" t="s">
-        <v>18</v>
-      </c>
+      <c r="I14" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="30">
+      <c r="A15" s="14">
+        <v>45662</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="24" customFormat="1" ht="30">
+      <c r="A16" s="21">
+        <v>45662</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="34" customFormat="1" ht="30">
+      <c r="A17" s="29">
+        <v>45662</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="H17" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="I17" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="24" customFormat="1" ht="60">
+      <c r="A18" s="21">
+        <v>45662</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="H18" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="I18" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="34" customFormat="1">
+      <c r="A19" s="29"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J3" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J3">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I3" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I3">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1443,22 +1709,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="68.44140625" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="68.42578125" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="20.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -1472,7 +1738,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="37.5">
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
@@ -1486,7 +1752,7 @@
         <v>45764</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="37.5">
       <c r="A3" s="5" t="s">
         <v>33</v>
       </c>
@@ -1500,7 +1766,7 @@
         <v>45768</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="18.75">
       <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
@@ -1514,7 +1780,7 @@
         <v>45776</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="37.5">
       <c r="A5" s="5" t="s">
         <v>35</v>
       </c>
@@ -1528,7 +1794,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="18.75">
       <c r="A6" s="5" t="s">
         <v>51</v>
       </c>
@@ -1542,7 +1808,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="74.400000000000006" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="75">
       <c r="A7" s="5" t="s">
         <v>75</v>
       </c>
@@ -1550,24 +1816,38 @@
         <v>32</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="D7" s="7">
         <v>45777</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="37.5">
       <c r="A8" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D8" s="19">
         <v>45777</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="37.5">
+      <c r="A9" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="19">
+        <v>45778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.8 close owner state for USERHOME  feature
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="6930" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="118">
   <si>
     <t>ID</t>
   </si>
@@ -509,6 +509,12 @@
   </si>
   <si>
     <t>Reviewed the 'Delete User' feature in the Admin Constraints section</t>
+  </si>
+  <si>
+    <t>v1.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">close owner state for USERHOME  feature </t>
   </si>
 </sst>
 </file>
@@ -1086,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1227,7 +1233,7 @@
         <v>41</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>18</v>
@@ -1259,7 +1265,7 @@
         <v>41</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="J5" s="15" t="s">
         <v>18</v>
@@ -1710,10 +1716,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1850,6 +1856,20 @@
         <v>45778</v>
       </c>
     </row>
+    <row r="10" spans="1:4" ht="18.75">
+      <c r="A10" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="19">
+        <v>45778</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
V1.9 update owner status for the delete user page
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="6930"/>
   </bookViews>
@@ -520,7 +520,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -870,7 +870,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -905,7 +905,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1082,7 +1082,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1092,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="G3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1585,7 +1585,7 @@
         <v>112</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="J15" s="15" t="s">
         <v>18</v>
@@ -1616,8 +1616,8 @@
       <c r="H16" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="I16" s="22" t="s">
-        <v>18</v>
+      <c r="I16" s="26" t="s">
+        <v>23</v>
       </c>
       <c r="J16" s="22" t="s">
         <v>18</v>
@@ -1648,8 +1648,8 @@
       <c r="H17" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="I17" s="33" t="s">
-        <v>18</v>
+      <c r="I17" s="30" t="s">
+        <v>23</v>
       </c>
       <c r="J17" s="33" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
v1.10 reviewed registration CRS
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="135">
   <si>
     <t>ID</t>
   </si>
@@ -516,11 +516,63 @@
   <si>
     <t xml:space="preserve">close owner state for USERHOME  feature </t>
   </si>
+  <si>
+    <t>v2.6</t>
+  </si>
+  <si>
+    <t>LH-CRS-REGISTRATION-008</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-016</t>
+  </si>
+  <si>
+    <t>this CRS is already mentioned in LH-CRS-REGISTRATION-005</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-017</t>
+  </si>
+  <si>
+    <t>LH-CRS-REGISTRATION-009</t>
+  </si>
+  <si>
+    <t>this CRS is already mentioned in LH-CRS-REGISTRATION-006</t>
+  </si>
+  <si>
+    <t>so we can be satisfied with the LH-CRS-REGISTRATION-005 and the constraints can be mentioned in SRS</t>
+  </si>
+  <si>
+    <t>so we can be satisfied with the LH-CRS-REGISTRATION-006 and any more details can be mentioned in SRS</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-018</t>
+  </si>
+  <si>
+    <t>LH-CRS-REGISTRATION-010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">you mention "as seen in the wireframe" </t>
+  </si>
+  <si>
+    <t>we don't need to mention that as CRS wrote before the 
+wireframe design an we can be satisfied by (All error messages must be displayed in a consistent and visible location, such as beneath the relevant input field or in a designated error message area)</t>
+  </si>
+  <si>
+    <t>v1.9</t>
+  </si>
+  <si>
+    <t>reviewed registration CRS</t>
+  </si>
+  <si>
+    <t>v1.10</t>
+  </si>
+  <si>
+    <t>update owner status</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -705,7 +757,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -808,6 +860,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -870,7 +925,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -905,7 +960,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1082,7 +1137,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1090,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1623,7 +1678,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="34" customFormat="1" ht="30">
+    <row r="17" spans="1:16" s="34" customFormat="1" ht="30">
       <c r="A17" s="29">
         <v>45662</v>
       </c>
@@ -1655,7 +1710,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="24" customFormat="1" ht="60">
+    <row r="18" spans="1:16" s="24" customFormat="1" ht="60">
       <c r="A18" s="21">
         <v>45662</v>
       </c>
@@ -1680,24 +1735,113 @@
       <c r="H18" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="I18" s="22" t="s">
+      <c r="I18" s="26" t="s">
         <v>18</v>
       </c>
       <c r="J18" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="34" customFormat="1">
-      <c r="A19" s="29"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
+    <row r="19" spans="1:16" s="34" customFormat="1" ht="30">
+      <c r="A19" s="29">
+        <v>45693</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="G19" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="30">
+      <c r="A20" s="21">
+        <v>45693</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="75">
+      <c r="A21" s="29">
+        <v>45693</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="H21" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="P21" s="35"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -1716,10 +1860,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1870,6 +2014,34 @@
         <v>45778</v>
       </c>
     </row>
+    <row r="11" spans="1:4" ht="18.75">
+      <c r="A11" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="19">
+        <v>45779</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18.75">
+      <c r="A12" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" s="19">
+        <v>45779</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v1.9 Reviewed publish Video and admin home
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F9C6BF-3901-4418-A12E-A1ED10A56C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="6930"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="133">
   <si>
     <t>ID</t>
   </si>
@@ -516,12 +517,58 @@
   <si>
     <t xml:space="preserve">close owner state for USERHOME  feature </t>
   </si>
+  <si>
+    <t>LH-CRS-Review-016</t>
+  </si>
+  <si>
+    <t>Omar Sherif</t>
+  </si>
+  <si>
+    <t>v2.6</t>
+  </si>
+  <si>
+    <t>Dropdown is present, but lacks confirmation/security details in description or wireframe.</t>
+  </si>
+  <si>
+    <t>Add confirmation and secure-action behavior to the description.</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LH-CRS-ADMINHOME-003	</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISHVIDEO-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix: capitalized "he" → "The" and smoothed out the sentence structure
+</t>
+  </si>
+  <si>
+    <t>(Fix: Changed “formats” to singular “format” since only .mp4 is allowed.</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISHVIDEO-003</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-017</t>
+  </si>
+  <si>
+    <t>LH-CRS-Review-018</t>
+  </si>
+  <si>
+    <t>v1.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reviewed publish Video and admin home  </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -705,7 +752,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -757,15 +804,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1082,36 +1120,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="12" customWidth="1"/>
-    <col min="6" max="6" width="66.140625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="55.85546875" style="12" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="66.109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="55.88671875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" style="12" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="10" customFormat="1" ht="18.75">
+    <row r="1" spans="1:10" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1143,7 +1181,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30">
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
@@ -1175,7 +1213,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="60">
+    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>14</v>
       </c>
@@ -1207,7 +1245,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="45">
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>24</v>
       </c>
@@ -1239,7 +1277,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30">
+    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>24</v>
       </c>
@@ -1271,7 +1309,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="45">
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>24</v>
       </c>
@@ -1303,7 +1341,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="60">
+    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>24</v>
       </c>
@@ -1335,7 +1373,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30">
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
@@ -1367,7 +1405,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="60">
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>24</v>
       </c>
@@ -1399,7 +1437,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
@@ -1431,7 +1469,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="45">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>24</v>
       </c>
@@ -1463,7 +1501,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="30">
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>24</v>
       </c>
@@ -1495,7 +1533,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="60">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>24</v>
       </c>
@@ -1527,39 +1565,39 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="24" customFormat="1" ht="30">
-      <c r="A14" s="25" t="s">
+    <row r="14" spans="1:10" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="G14" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="H14" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="I14" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="30">
+      <c r="I14" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
         <v>45662</v>
       </c>
@@ -1591,121 +1629,217 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="24" customFormat="1" ht="30">
-      <c r="A16" s="21">
+    <row r="16" spans="1:10" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="18">
         <v>45662</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="H16" s="28" t="s">
+      <c r="H16" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="I16" s="26" t="s">
+      <c r="I16" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="34" customFormat="1" ht="30">
-      <c r="A17" s="29">
+      <c r="J16" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="31" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="26">
         <v>45662</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="H17" s="32" t="s">
+      <c r="H17" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="I17" s="30" t="s">
+      <c r="I17" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="24" customFormat="1" ht="60">
-      <c r="A18" s="21">
+      <c r="J17" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="21" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="18">
         <v>45662</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="26" t="s">
+      <c r="E18" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="G18" s="27" t="s">
+      <c r="G18" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="H18" s="28" t="s">
+      <c r="H18" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="I18" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18" s="22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="34" customFormat="1">
-      <c r="A19" s="29"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
+      <c r="I18" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="18">
+        <v>45693</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="21" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="18">
+        <v>45693</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="18">
+        <v>45693</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="26"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J3">
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I3" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1715,22 +1849,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="68.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="68.44140625" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25">
+    <row r="1" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -1744,7 +1878,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="37.5">
+    <row r="2" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
@@ -1758,7 +1892,7 @@
         <v>45764</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="37.5">
+    <row r="3" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>33</v>
       </c>
@@ -1772,7 +1906,7 @@
         <v>45768</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75">
+    <row r="4" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
@@ -1786,7 +1920,7 @@
         <v>45776</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="37.5">
+    <row r="5" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>35</v>
       </c>
@@ -1800,7 +1934,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18.75">
+    <row r="6" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>51</v>
       </c>
@@ -1814,7 +1948,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="75">
+    <row r="7" spans="1:4" ht="74.400000000000006" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>75</v>
       </c>
@@ -1828,46 +1962,60 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="37.5">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="7">
         <v>45777</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="37.5">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="7">
         <v>45778</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18.75">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="7">
         <v>45778</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="7">
+        <v>45779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v2.3 Change owner state for ADMIN HOME and PUBLISH VIDEO features
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_CRS_REVIEWS.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640ECA85-EB05-486E-A352-6A55A0F9A0A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="REVIEW-SHEET" sheetId="3" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="147">
   <si>
     <t>ID</t>
   </si>
@@ -78,9 +77,6 @@
   </si>
   <si>
     <t>open</t>
-  </si>
-  <si>
-    <t>Omar</t>
   </si>
   <si>
     <t xml:space="preserve">At notification feature the CRS is too vauge and does not explain what the customer want the system do </t>
@@ -145,9 +141,6 @@
   </si>
   <si>
     <t>it can only be "The home page must dynamically fetch and display notifications for new articles in categories the user follows"</t>
-  </si>
-  <si>
-    <t>hala</t>
   </si>
   <si>
     <t>LH-CRS-Review-004</t>
@@ -515,9 +508,6 @@
     <t>v1.8</t>
   </si>
   <si>
-    <t xml:space="preserve">close owner state for USERHOME  feature </t>
-  </si>
-  <si>
     <t>LH-CRS-Review-016</t>
   </si>
   <si>
@@ -567,13 +557,7 @@
     <t>update owner status</t>
   </si>
   <si>
-    <t>v1.10</t>
-  </si>
-  <si>
     <t>reviewed registration CRS</t>
-  </si>
-  <si>
-    <t>v1.11</t>
   </si>
   <si>
     <t>LH-CRS-REGISTRATION-008</t>
@@ -610,13 +594,22 @@
     <t>Closed review on Publish audio</t>
   </si>
   <si>
-    <t>v1.12</t>
+    <t>not applicable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close owner state for USERHOME  feature </t>
+  </si>
+  <si>
+    <t>Change owner state for ADMIN HOME and PUBLISH VIDEO features</t>
+  </si>
+  <si>
+    <t>v2.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -957,7 +950,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -992,7 +985,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1176,11 +1169,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView topLeftCell="D9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="E16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1206,7 +1199,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>1</v>
@@ -1235,10 +1228,10 @@
         <v>14</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>15</v>
@@ -1247,19 +1240,19 @@
         <v>16</v>
       </c>
       <c r="F2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="16" t="s">
-        <v>38</v>
-      </c>
       <c r="H2" s="11" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="60">
@@ -1267,10 +1260,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>15</v>
@@ -1279,48 +1272,48 @@
         <v>17</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="45">
       <c r="A4" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>32</v>
-      </c>
       <c r="E4" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>18</v>
@@ -1328,31 +1321,31 @@
     </row>
     <row r="5" spans="1:10" ht="30">
       <c r="A5" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>44</v>
-      </c>
       <c r="H5" s="15" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J5" s="15" t="s">
         <v>18</v>
@@ -1360,31 +1353,31 @@
     </row>
     <row r="6" spans="1:10" ht="45">
       <c r="A6" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>59</v>
-      </c>
       <c r="G6" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J6" s="11" t="s">
         <v>18</v>
@@ -1392,31 +1385,31 @@
     </row>
     <row r="7" spans="1:10" ht="60">
       <c r="A7" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="D7" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>60</v>
-      </c>
       <c r="G7" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J7" s="15" t="s">
         <v>18</v>
@@ -1424,31 +1417,31 @@
     </row>
     <row r="8" spans="1:10" ht="30">
       <c r="A8" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>63</v>
-      </c>
       <c r="D8" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>54</v>
-      </c>
       <c r="F8" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>18</v>
@@ -1456,31 +1449,31 @@
     </row>
     <row r="9" spans="1:10" ht="60">
       <c r="A9" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D9" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>54</v>
-      </c>
       <c r="F9" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="17" t="s">
-        <v>70</v>
-      </c>
       <c r="H9" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J9" s="15" t="s">
         <v>18</v>
@@ -1488,31 +1481,31 @@
     </row>
     <row r="10" spans="1:10" ht="30">
       <c r="A10" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>73</v>
-      </c>
       <c r="H10" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>18</v>
@@ -1520,31 +1513,31 @@
     </row>
     <row r="11" spans="1:10" ht="45">
       <c r="A11" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="17" t="s">
-        <v>83</v>
-      </c>
       <c r="G11" s="17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J11" s="15" t="s">
         <v>18</v>
@@ -1552,31 +1545,31 @@
     </row>
     <row r="12" spans="1:10" ht="30">
       <c r="A12" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="11" t="s">
+      <c r="F12" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="16" t="s">
-        <v>83</v>
-      </c>
       <c r="G12" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>18</v>
@@ -1584,31 +1577,31 @@
     </row>
     <row r="13" spans="1:10" ht="60">
       <c r="A13" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J13" s="15" t="s">
         <v>18</v>
@@ -1616,31 +1609,31 @@
     </row>
     <row r="14" spans="1:10" s="21" customFormat="1" ht="30">
       <c r="A14" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="E14" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="G14" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="E14" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>91</v>
-      </c>
       <c r="H14" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I14" s="23" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="J14" s="19" t="s">
         <v>18</v>
@@ -1651,28 +1644,28 @@
         <v>45662</v>
       </c>
       <c r="B15" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>98</v>
-      </c>
       <c r="D15" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F15" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="G15" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>112</v>
-      </c>
       <c r="I15" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J15" s="15" t="s">
         <v>18</v>
@@ -1683,28 +1676,28 @@
         <v>45662</v>
       </c>
       <c r="B16" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="D16" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>101</v>
-      </c>
       <c r="H16" s="25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J16" s="19" t="s">
         <v>18</v>
@@ -1715,28 +1708,28 @@
         <v>45662</v>
       </c>
       <c r="B17" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C17" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="F17" s="28" t="s">
-        <v>104</v>
-      </c>
       <c r="G17" s="28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H17" s="29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I17" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J17" s="30" t="s">
         <v>18</v>
@@ -1747,25 +1740,25 @@
         <v>45662</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I18" s="19" t="s">
         <v>18</v>
@@ -1779,31 +1772,31 @@
         <v>45693</v>
       </c>
       <c r="B19" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="C19" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="D19" s="27" t="s">
+      <c r="G19" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="H19" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="J19" s="30" t="s">
         <v>120</v>
-      </c>
-      <c r="F19" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="G19" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="H19" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="I19" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="J19" s="30" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="21" customFormat="1" ht="45">
@@ -1811,31 +1804,31 @@
         <v>45693</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E20" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="19" t="s">
         <v>120</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="H20" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="I20" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="J20" s="19" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="21" customFormat="1" ht="30">
@@ -1843,31 +1836,31 @@
         <v>45693</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E21" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="I21" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="30" t="s">
         <v>120</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="G21" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="H21" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="I21" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="30" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="31" customFormat="1" ht="30">
@@ -1875,25 +1868,25 @@
         <v>45693</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I22" s="23" t="s">
         <v>18</v>
@@ -1907,25 +1900,25 @@
         <v>45693</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="H23" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I23" s="27" t="s">
         <v>18</v>
@@ -1939,25 +1932,25 @@
         <v>45693</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I24" s="23" t="s">
         <v>18</v>
@@ -1969,10 +1962,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J3" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="choose from list" sqref="J2:J3">
       <formula1>"open,closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I3" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="select from list" sqref="I2:I3">
       <formula1>"open,in progress,closed,not applicable"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1982,11 +1975,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2016,10 +2009,10 @@
         <v>13</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="D2" s="7">
         <v>45764</v>
@@ -2027,13 +2020,13 @@
     </row>
     <row r="3" spans="1:4" ht="37.5">
       <c r="A3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" s="7">
         <v>45768</v>
@@ -2041,13 +2034,13 @@
     </row>
     <row r="4" spans="1:4" ht="18.75">
       <c r="A4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D4" s="7">
         <v>45776</v>
@@ -2055,13 +2048,13 @@
     </row>
     <row r="5" spans="1:4" ht="37.5">
       <c r="A5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D5" s="7">
         <v>45777</v>
@@ -2069,13 +2062,13 @@
     </row>
     <row r="6" spans="1:4" ht="18.75">
       <c r="A6" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D6" s="7">
         <v>45777</v>
@@ -2083,13 +2076,13 @@
     </row>
     <row r="7" spans="1:4" ht="75">
       <c r="A7" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D7" s="7">
         <v>45777</v>
@@ -2097,13 +2090,13 @@
     </row>
     <row r="8" spans="1:4" ht="37.5">
       <c r="A8" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D8" s="7">
         <v>45777</v>
@@ -2111,13 +2104,13 @@
     </row>
     <row r="9" spans="1:4" ht="37.5">
       <c r="A9" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D9" s="7">
         <v>45778</v>
@@ -2125,13 +2118,13 @@
     </row>
     <row r="10" spans="1:4" ht="18.75">
       <c r="A10" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>117</v>
+        <v>144</v>
       </c>
       <c r="D10" s="7">
         <v>45778</v>
@@ -2139,13 +2132,13 @@
     </row>
     <row r="11" spans="1:4" ht="18.75">
       <c r="A11" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D11" s="7">
         <v>45779</v>
@@ -2153,13 +2146,13 @@
     </row>
     <row r="12" spans="1:4" ht="18.75">
       <c r="A12" s="5" t="s">
-        <v>134</v>
+        <v>51</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D12" s="7">
         <v>45779</v>
@@ -2167,13 +2160,13 @@
     </row>
     <row r="13" spans="1:4" ht="18.75">
       <c r="A13" s="5" t="s">
-        <v>136</v>
+        <v>52</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D13" s="7">
         <v>45779</v>
@@ -2181,15 +2174,29 @@
     </row>
     <row r="14" spans="1:4" ht="18.75">
       <c r="A14" s="5" t="s">
-        <v>148</v>
+        <v>79</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D14" s="7">
+        <v>45781</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="37.5">
+      <c r="A15" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" s="7">
         <v>45781</v>
       </c>
     </row>

</xml_diff>